<commit_message>
Update Test Cases with one more failed test
</commit_message>
<xml_diff>
--- a/Test Cases Web Project.xlsx
+++ b/Test Cases Web Project.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29721"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAE33EE8-750F-491E-8206-52628FC13192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2798ED5B-8E7F-4A91-BDFB-F696E26126DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
   <si>
     <t xml:space="preserve"> Test Case ID</t>
   </si>
@@ -201,7 +201,7 @@
     <t>System applies security measures(captcha/temporary lock)</t>
   </si>
   <si>
-    <t>After multiple failed login attempts, a captcha challenge was triggered</t>
+    <t>Login attempts allowed indefinitely with no captcha or account lock</t>
   </si>
   <si>
     <t>Security</t>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t>Registration was blocked and a validation message was displayed indicating that the username is already taken</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <t>Login/Register</t>
   </si>
 </sst>
 </file>
@@ -543,11 +549,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -586,7 +589,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -594,44 +596,234 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -640,156 +832,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1107,698 +1149,763 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7:T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="22.5" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="64"/>
-      <c r="F1" s="63" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="57" t="s">
+      <c r="G1" s="59"/>
+      <c r="H1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="58"/>
-      <c r="J1" s="31" t="s">
+      <c r="I1" s="51"/>
+      <c r="J1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="31" t="s">
+      <c r="K1" s="52"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="31" t="s">
+      <c r="N1" s="52"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="11" t="s">
+      <c r="Q1" s="52"/>
+      <c r="R1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="S1" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="33"/>
+      <c r="T1" s="95"/>
       <c r="U1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="81" customHeight="1">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="35" t="s">
+      <c r="E2" s="61"/>
+      <c r="F2" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="61"/>
+      <c r="H2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="65"/>
-      <c r="J2" s="66" t="s">
+      <c r="I2" s="63"/>
+      <c r="J2" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="67"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="60" t="s">
+      <c r="K2" s="65"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="61"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="20" t="s">
+      <c r="N2" s="55"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="13" t="s">
+      <c r="Q2" s="92"/>
+      <c r="R2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="34" t="s">
+      <c r="S2" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="34"/>
-      <c r="U2" s="14" t="s">
+      <c r="T2" s="96"/>
+      <c r="U2" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="6" customFormat="1" ht="72.75" customHeight="1">
-      <c r="A3" s="55" t="s">
+    <row r="3" spans="1:21" s="5" customFormat="1" ht="72.75" customHeight="1">
+      <c r="A3" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="77"/>
+      <c r="F3" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="70" t="s">
+      <c r="G3" s="62"/>
+      <c r="H3" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="39" t="s">
+      <c r="I3" s="70"/>
+      <c r="J3" s="71" t="s">
         <v>25</v>
       </c>
       <c r="K3" s="72"/>
       <c r="L3" s="73"/>
-      <c r="M3" s="42" t="s">
+      <c r="M3" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="74"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="20" t="s">
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="18" t="s">
+      <c r="Q3" s="45"/>
+      <c r="R3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="22" t="s">
+      <c r="S3" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="23"/>
-      <c r="U3" s="14" t="s">
+      <c r="T3" s="91"/>
+      <c r="U3" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="84.75" customHeight="1">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="57"/>
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="35" t="s">
+      <c r="E4" s="78"/>
+      <c r="F4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="20" t="s">
+      <c r="G4" s="62"/>
+      <c r="H4" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="69" t="s">
+      <c r="I4" s="45"/>
+      <c r="J4" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="69"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="24" t="s">
+      <c r="K4" s="67"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="25"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="27" t="s">
+      <c r="N4" s="39"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="19" t="s">
+      <c r="Q4" s="37"/>
+      <c r="R4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="29" t="s">
+      <c r="S4" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="T4" s="30"/>
-      <c r="U4" s="15" t="s">
+      <c r="T4" s="41"/>
+      <c r="U4" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="102.75" customHeight="1">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="57"/>
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="35" t="s">
+      <c r="E5" s="76"/>
+      <c r="F5" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="20" t="s">
+      <c r="G5" s="62"/>
+      <c r="H5" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="24" t="s">
+      <c r="I5" s="37"/>
+      <c r="J5" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="76"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="24" t="s">
+      <c r="K5" s="47"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="25"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="20" t="s">
+      <c r="N5" s="39"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="12" t="s">
+      <c r="Q5" s="37"/>
+      <c r="R5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="79" t="s">
+      <c r="S5" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="30"/>
-      <c r="U5" s="15" t="s">
+      <c r="T5" s="41"/>
+      <c r="U5" s="14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="8" customFormat="1" ht="99.75" customHeight="1">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:21" s="7" customFormat="1" ht="99.75" customHeight="1">
+      <c r="A6" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="57"/>
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="37" t="s">
+      <c r="E6" s="79"/>
+      <c r="F6" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="20" t="s">
+      <c r="G6" s="32"/>
+      <c r="H6" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="24" t="s">
+      <c r="I6" s="37"/>
+      <c r="J6" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="76"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="24" t="s">
+      <c r="K6" s="47"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="N6" s="25"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="20" t="s">
+      <c r="N6" s="39"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="12" t="s">
+      <c r="Q6" s="37"/>
+      <c r="R6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="S6" s="79" t="s">
+      <c r="S6" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="T6" s="30"/>
-      <c r="U6" s="15" t="s">
+      <c r="T6" s="41"/>
+      <c r="U6" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="65.25" customHeight="1">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="46"/>
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="24" t="s">
+      <c r="E7" s="49"/>
+      <c r="F7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="20" t="s">
+      <c r="G7" s="34"/>
+      <c r="H7" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="24" t="s">
+      <c r="I7" s="37"/>
+      <c r="J7" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="76"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="24" t="s">
+      <c r="K7" s="47"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="N7" s="25"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="20" t="s">
+      <c r="N7" s="39"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="S7" s="79" t="s">
+      <c r="Q7" s="37"/>
+      <c r="R7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="T7" s="30"/>
-      <c r="U7" s="15" t="s">
+      <c r="T7" s="41"/>
+      <c r="U7" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="90.75" customHeight="1">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="57"/>
+      <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="39" t="s">
+      <c r="E8" s="82"/>
+      <c r="F8" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="40"/>
-      <c r="H8" s="20" t="s">
+      <c r="G8" s="81"/>
+      <c r="H8" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="28"/>
-      <c r="J8" s="24" t="s">
+      <c r="I8" s="37"/>
+      <c r="J8" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="76"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="24" t="s">
+      <c r="K8" s="47"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="25"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="20" t="s">
+      <c r="N8" s="39"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="12" t="s">
+      <c r="Q8" s="37"/>
+      <c r="R8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="S8" s="80" t="s">
+      <c r="S8" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="T8" s="81"/>
-      <c r="U8" s="16" t="s">
+      <c r="T8" s="44"/>
+      <c r="U8" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="78" customHeight="1">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="46"/>
+      <c r="C9" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="20" t="s">
+      <c r="E9" s="80"/>
+      <c r="F9" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="20" t="s">
+      <c r="G9" s="37"/>
+      <c r="H9" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="82" t="s">
+      <c r="I9" s="37"/>
+      <c r="J9" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="24" t="s">
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="N9" s="25"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="20" t="s">
+      <c r="N9" s="39"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="17" t="s">
+      <c r="Q9" s="37"/>
+      <c r="R9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="S9" s="80" t="s">
+      <c r="S9" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="T9" s="81"/>
-      <c r="U9" s="15" t="s">
+      <c r="T9" s="44"/>
+      <c r="U9" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="105" customHeight="1">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="46"/>
+      <c r="C10" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="20" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="20" t="s">
+      <c r="G10" s="37"/>
+      <c r="H10" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="53" t="s">
+      <c r="I10" s="45"/>
+      <c r="J10" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="76" t="s">
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="N10" s="25"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="20" t="s">
+      <c r="N10" s="39"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="17" t="s">
+      <c r="Q10" s="37"/>
+      <c r="R10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="79" t="s">
+      <c r="S10" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="T10" s="30"/>
-      <c r="U10" s="15" t="s">
+      <c r="T10" s="41"/>
+      <c r="U10" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="92.25" customHeight="1">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="57"/>
+      <c r="C11" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="35" t="s">
+      <c r="E11" s="37"/>
+      <c r="F11" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="20" t="s">
+      <c r="G11" s="62"/>
+      <c r="H11" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="28"/>
-      <c r="J11" s="44" t="s">
+      <c r="I11" s="37"/>
+      <c r="J11" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="45"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="24" t="s">
+      <c r="K11" s="35"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="N11" s="25"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="20" t="s">
+      <c r="N11" s="39"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="12" t="s">
+      <c r="Q11" s="37"/>
+      <c r="R11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="S11" s="79" t="s">
+      <c r="S11" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="T11" s="30"/>
-      <c r="U11" s="15" t="s">
+      <c r="T11" s="41"/>
+      <c r="U11" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="85.5" customHeight="1">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="57"/>
+      <c r="C12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="35" t="s">
+      <c r="E12" s="37"/>
+      <c r="F12" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="20" t="s">
+      <c r="G12" s="62"/>
+      <c r="H12" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="44" t="s">
+      <c r="I12" s="37"/>
+      <c r="J12" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="45"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="24" t="s">
+      <c r="K12" s="35"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="N12" s="25"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="20" t="s">
+      <c r="N12" s="39"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="12" t="s">
+      <c r="Q12" s="37"/>
+      <c r="R12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="S12" s="80" t="s">
+      <c r="S12" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="T12" s="81"/>
-      <c r="U12" s="15" t="s">
+      <c r="T12" s="44"/>
+      <c r="U12" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="93" customHeight="1">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="35" t="s">
+      <c r="E13" s="89"/>
+      <c r="F13" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="83" t="s">
+      <c r="G13" s="62"/>
+      <c r="H13" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="I13" s="28"/>
-      <c r="J13" s="44" t="s">
+      <c r="I13" s="37"/>
+      <c r="J13" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="K13" s="45"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="24" t="s">
+      <c r="K13" s="35"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="20" t="s">
+      <c r="N13" s="39"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="12" t="s">
+      <c r="Q13" s="37"/>
+      <c r="R13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="S13" s="79" t="s">
+      <c r="S13" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="T13" s="30"/>
-      <c r="U13" s="15" t="s">
+      <c r="T13" s="41"/>
+      <c r="U13" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="96" customHeight="1">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="45"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="47"/>
-      <c r="F14" s="48" t="s">
+      <c r="E14" s="86"/>
+      <c r="F14" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="20" t="s">
+      <c r="G14" s="88"/>
+      <c r="H14" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="28"/>
-      <c r="J14" s="84" t="s">
+      <c r="I14" s="24"/>
+      <c r="J14" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="24" t="s">
+      <c r="K14" s="28"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="N14" s="25"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="20" t="s">
+      <c r="N14" s="28"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="12" t="s">
+      <c r="Q14" s="24"/>
+      <c r="R14" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="S14" s="79" t="s">
+      <c r="S14" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="T14" s="30"/>
-      <c r="U14" s="15" t="s">
+      <c r="T14" s="26"/>
+      <c r="U14" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="13:13">
-      <c r="M17" s="1"/>
+    <row r="15" spans="1:21" ht="47.25" customHeight="1">
+      <c r="A15" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="112">
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="S7:T7"/>
+  <mergeCells count="120">
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M2:O2"/>
@@ -1823,47 +1930,61 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="S15:T15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>